<commit_message>
Improve and protect calculation sheet
</commit_message>
<xml_diff>
--- a/dimensions.xlsx
+++ b/dimensions.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Makerspace\water-bottles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Makerspace\ignite-bottles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA75064B-1E88-4223-BAB3-EA21653BC308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9C53ED-2283-4124-94F5-79CBF3B55BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63FF3512-A52B-4B37-9E24-F61970BC3DDB}"/>
   </bookViews>
@@ -32,30 +32,147 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nick</author>
+  </authors>
+  <commentList>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6583F5DB-9463-4C6C-91F5-9F661D20DD88}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Plug these into the coords for the inkscape object. Assumes that the bottle is perfectly centered, facing up in the laser bed.
+X=0 ==&gt; base of bottle
+Y=0 ==&gt; start of rotation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{E0D28D42-E06F-458A-9E9D-3ACA1B7F660D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Height from offset, needs to be manually determined. This is just the "H for offset from start" value. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{4704C482-8C91-425A-9D42-9723652170D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the Y for the logo when centered on the back of the bottle.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{CF65677C-E218-4A84-ABE5-6320FD28D4EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Centers logo at the height listed in "H for centering" cell.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{CA5D5FDE-722A-44C0-9B0B-05D8BEEBAC77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the Y of the logo when it is centered on front of the bottle.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Bottle D</t>
-  </si>
-  <si>
-    <t>Bottle C/2</t>
-  </si>
-  <si>
-    <t>Logo Width</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Logo Midx</t>
   </si>
   <si>
-    <t>Logo Y</t>
-  </si>
-  <si>
     <t>Logo Midy</t>
   </si>
   <si>
-    <t>Logo W/H</t>
-  </si>
-  <si>
     <t>INPUTS</t>
   </si>
   <si>
@@ -65,32 +182,59 @@
     <t>INKSCAPE VALUES</t>
   </si>
   <si>
-    <t>Height From Curve</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Doc H</t>
-  </si>
-  <si>
-    <t>Doc W</t>
+    <t>BOTTLE</t>
+  </si>
+  <si>
+    <t>INKSCAPE GRAPHIC</t>
+  </si>
+  <si>
+    <t>Circumfrence</t>
+  </si>
+  <si>
+    <t>C/2</t>
+  </si>
+  <si>
+    <t>Y (opposite side)</t>
+  </si>
+  <si>
+    <t>Y (full rotation)</t>
+  </si>
+  <si>
+    <t>X (centered)</t>
+  </si>
+  <si>
+    <t>X (from start)</t>
+  </si>
+  <si>
+    <t>H for centering</t>
+  </si>
+  <si>
+    <t>H for offset from start</t>
+  </si>
+  <si>
+    <t>Bottle diameter</t>
+  </si>
+  <si>
+    <t>Logo width</t>
+  </si>
+  <si>
+    <t>Logo height</t>
+  </si>
+  <si>
+    <t>MM --&gt; IN</t>
+  </si>
+  <si>
+    <t>IN --&gt; MM</t>
+  </si>
+  <si>
+    <t>CONVERT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,13 +250,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,12 +305,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,6 +357,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8936</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C028389-FC30-4DEC-94DB-43B483B5901A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="2695575"/>
+          <a:ext cx="3971335" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,144 +713,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68894AED-1E70-4DAD-AF38-55BE706A3966}">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68894AED-1E70-4DAD-AF38-55BE706A3966}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="G2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="H1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="11">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.375</v>
+      </c>
+      <c r="D3" s="11">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <f>(B3*PI())</f>
+        <v>9.4247779607693793</v>
+      </c>
+      <c r="G3" s="13">
+        <f>F3/2</f>
+        <v>4.7123889803846897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6">
+        <f>CONVERT(E3,"in", "mm")</f>
+        <v>25.4</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11">
+        <v>4.25</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.887</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13">
+        <f>B5/2</f>
+        <v>2.125</v>
+      </c>
+      <c r="G5" s="13">
+        <f>C5/2</f>
+        <v>0.94350000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="E7" s="6">
+        <f>CONVERT(E6,"mm", "in")</f>
+        <v>3.937007874015748E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>C3</f>
+        <v>1.375</v>
+      </c>
+      <c r="B9">
+        <f>G3-G5</f>
+        <v>3.7688889803846894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1.375</v>
-      </c>
-      <c r="D3">
-        <f>(A3*PI())/2</f>
-        <v>4.7123889803846897</v>
-      </c>
-      <c r="H3">
-        <f>B3</f>
-        <v>1.375</v>
-      </c>
-      <c r="I3">
-        <f>D3-F5</f>
-        <v>3.7687832965480998</v>
-      </c>
-      <c r="J3">
-        <f>A5</f>
-        <v>4.25</v>
-      </c>
-      <c r="K3">
-        <f>E5</f>
-        <v>1.8872113676731797</v>
-      </c>
-      <c r="L3">
-        <f>H3+J3</f>
-        <v>5.625</v>
-      </c>
-      <c r="M3">
-        <f>I3+K3</f>
-        <v>5.6559946642212795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4.25</v>
-      </c>
-      <c r="B5">
-        <v>2.2519999999999998</v>
-      </c>
-      <c r="D5">
-        <f>A5/2</f>
-        <v>2.125</v>
-      </c>
-      <c r="E5">
-        <f>A5/B5</f>
-        <v>1.8872113676731797</v>
-      </c>
-      <c r="F5">
-        <f>E5/2</f>
-        <v>0.94360568383658983</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>D3-G5</f>
+        <v>4.0564999999999998</v>
+      </c>
+      <c r="B11">
+        <f>F3-G5</f>
+        <v>8.4812779607693791</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:B1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zqrlc/M7V22KQHxDnsVI0w49foVH8gtaOMs/HcipMGKBQQWcrpYmd8D9xXDosV0u5iaPaFPgSxYlzy1kBnYlCQ==" saltValue="E8dMdSjjHSVJoS+K96Fi2A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>